<commit_message>
modify row-title judging standard
</commit_message>
<xml_diff>
--- a/test/output.xlsx
+++ b/test/output.xlsx
@@ -405,10 +405,10 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>样地1</v>
+        <v>A1</v>
       </c>
       <c r="B2" t="str">
-        <v>A</v>
+        <v>松树</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -431,10 +431,10 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>样地1</v>
+        <v>A1</v>
       </c>
       <c r="B3" t="str">
-        <v>B</v>
+        <v>杨树</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -457,10 +457,10 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>样地1</v>
+        <v>A1</v>
       </c>
       <c r="B4" t="str">
-        <v>C</v>
+        <v>柳树</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -483,10 +483,10 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>样地2</v>
+        <v>A2</v>
       </c>
       <c r="B5" t="str">
-        <v>A</v>
+        <v>松树</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -509,10 +509,10 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>样地2</v>
+        <v>A2</v>
       </c>
       <c r="B6" t="str">
-        <v>C</v>
+        <v>柳树</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -569,7 +569,7 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>A</v>
+        <v>松树</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -595,7 +595,7 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>B</v>
+        <v>杨树</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -621,7 +621,7 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>C</v>
+        <v>柳树</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -666,7 +666,7 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>样地1</v>
+        <v>A1</v>
       </c>
       <c r="B2">
         <v>3</v>
@@ -677,7 +677,7 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>样地2</v>
+        <v>A2</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -722,10 +722,10 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>样地1</v>
+        <v>A1</v>
       </c>
       <c r="B2" t="str">
-        <v>A</v>
+        <v>松树</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -748,10 +748,10 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>样地1</v>
+        <v>A1</v>
       </c>
       <c r="B3" t="str">
-        <v>B</v>
+        <v>杨树</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -774,10 +774,10 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>样地1</v>
+        <v>A1</v>
       </c>
       <c r="B4" t="str">
-        <v>C</v>
+        <v>柳树</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -800,10 +800,10 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>样地2</v>
+        <v>A2</v>
       </c>
       <c r="B5" t="str">
-        <v>A</v>
+        <v>松树</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -826,10 +826,10 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>样地2</v>
+        <v>A2</v>
       </c>
       <c r="B6" t="str">
-        <v>C</v>
+        <v>柳树</v>
       </c>
       <c r="C6">
         <v>1</v>

</xml_diff>

<commit_message>
Make category modifiable Change title type judging strategy
</commit_message>
<xml_diff>
--- a/test/output.xlsx
+++ b/test/output.xlsx
@@ -10,7 +10,6 @@
     <sheet name="大样地乔木层5" sheetId="5" r:id="rId5"/>
     <sheet name="大样地乔木层6" sheetId="6" r:id="rId6"/>
     <sheet name="大样地乔木层7" sheetId="7" r:id="rId7"/>
-    <sheet name="Sheet1" sheetId="8" r:id="rId8"/>
   </sheets>
 </workbook>
 </file>
@@ -5523,77 +5522,4 @@
     </row>
   </sheetData>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U1"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>物种</v>
-      </c>
-      <c r="B1" t="str">
-        <v>样方/种</v>
-      </c>
-      <c r="C1" t="str">
-        <v>总样方数</v>
-      </c>
-      <c r="D1" t="str">
-        <v>数量/种</v>
-      </c>
-      <c r="E1" t="str">
-        <v>总数量</v>
-      </c>
-      <c r="F1" t="str">
-        <v>胸高断/种</v>
-      </c>
-      <c r="G1" t="str">
-        <v>总胸高断</v>
-      </c>
-      <c r="H1" t="str">
-        <v>相对密度</v>
-      </c>
-      <c r="I1" t="str">
-        <v>相对频度</v>
-      </c>
-      <c r="J1" t="str">
-        <v>相对优势</v>
-      </c>
-      <c r="K1" t="str">
-        <v>重要值</v>
-      </c>
-      <c r="L1" t="str">
-        <v>Pi</v>
-      </c>
-      <c r="M1" t="str">
-        <v>lnPi</v>
-      </c>
-      <c r="N1" t="str">
-        <v>Pi*lnPi</v>
-      </c>
-      <c r="O1" t="str">
-        <v>分种Shannon-Wiener指数</v>
-      </c>
-      <c r="P1" t="str">
-        <v>Shannon-Wiener指数</v>
-      </c>
-      <c r="Q1" t="str">
-        <v>Pi2</v>
-      </c>
-      <c r="R1" t="str">
-        <v>Simpson指数</v>
-      </c>
-      <c r="S1" t="str">
-        <v>物种多样性指数</v>
-      </c>
-      <c r="T1" t="str">
-        <v>lnS</v>
-      </c>
-      <c r="U1" t="str">
-        <v>物种均匀度指数</v>
-      </c>
-    </row>
-  </sheetData>
-</worksheet>
 </file>
</xml_diff>